<commit_message>
se cambio url axios para la comunicacion con el backend en linea
</commit_message>
<xml_diff>
--- a/server/Datos_Formulario.xlsx
+++ b/server/Datos_Formulario.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803C77C2-4F11-458C-B1D6-37F20421C943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="Datos" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Datos" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -38,44 +34,39 @@
     <t>Modelos de autos</t>
   </si>
   <si>
-    <t>prueba</t>
-  </si>
-  <si>
-    <t>soccer</t>
-  </si>
-  <si>
-    <t>No estoy seguro</t>
-  </si>
-  <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>Nissan, Toyota</t>
-  </si>
-  <si>
-    <t>prueba2</t>
-  </si>
-  <si>
-    <t>Kansas</t>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>CORADO</t>
+  </si>
+  <si>
+    <t>Fútbol</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Toyota</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -100,31 +91,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,14 +445,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
@@ -478,7 +455,7 @@
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,84 +478,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>